<commit_message>
cenários com navio de 1900
</commit_message>
<xml_diff>
--- a/Resultados/CEN03.xlsx
+++ b/Resultados/CEN03.xlsx
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>262315</v>
+        <v>681000</v>
       </c>
     </row>
     <row r="5">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.4993919524236128</v>
+        <v>0.1923612334801762</v>
       </c>
     </row>
   </sheetData>

</xml_diff>